<commit_message>
poprawka i badania avl
</commit_message>
<xml_diff>
--- a/Pomiary.xlsx
+++ b/Pomiary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\studia\SEM 4\Struktury danych\Projekt3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B756B889-CD16-4021-86D2-33FB4B4D06A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21AD155-D3E9-4AE3-BF42-55A34443F994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5BA449A7-E08B-42BB-ABCF-9D574EF15BCC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{5BA449A7-E08B-42BB-ABCF-9D574EF15BCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablica dynamiczna" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>insert</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>metoda/rozmiar</t>
+  </si>
+  <si>
+    <t>AVL</t>
   </si>
 </sst>
 </file>
@@ -107,10 +110,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1427,6 +1430,633 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
+              <a:t>AVL</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>insert</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>AVL!$C$3:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>AVL!$C$4:$K$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>52.51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57.95</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72.650000000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60.32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67.27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>73.78</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66.69</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>66.290000000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A61C-4194-9F07-128068BCD7C5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>remove</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>AVL!$C$3:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>AVL!$C$5:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>63.68</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81.39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99.32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105.94</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>144.51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>198.84</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>260.05</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260.27999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A61C-4194-9F07-128068BCD7C5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1137594719"/>
+        <c:axId val="1137578399"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1137594719"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Rozmiar struktury</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1137578399"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1137578399"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Czas</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> [ns]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1137594719"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
               <a:t>Insert</a:t>
             </a:r>
           </a:p>
@@ -1682,6 +2312,115 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-53F2-40D2-B103-1E4236417EEB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>AVL</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>AVL!$C$3:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>AVL!$C$4:$K$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>52.51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57.95</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72.650000000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60.32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67.27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>73.78</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66.69</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>66.290000000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6F4B-4C59-9925-2C1994FFACEE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2019,7 +2758,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
@@ -2309,6 +3048,115 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C81B-476A-AD16-AC18B8A860BA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>AVL</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>AVL!$C$3:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>AVL!$C$5:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>63.68</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81.39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99.32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105.94</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>144.51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>198.84</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>260.05</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260.27999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FE20-41B3-AA60-6E6989FB3CEF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2806,6 +3654,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4355,6 +5243,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4953,6 +6357,47 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{345415EB-BBDA-9416-3899-015F5DA29E72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5351,7 +6796,7 @@
   <dimension ref="B2:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:K5"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5360,112 +6805,112 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>5000</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>8000</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>10000</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>16000</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>20000</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>40000</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>60000</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>80000</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <v>100000</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>28.98</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>29.82</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>28.84</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>30.49</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>33.159999999999997</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>34.01</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>34.549999999999997</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>33.51</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <v>34.15</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>30.58</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>29.67</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>30.02</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>29.22</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>28.85</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>34.630000000000003</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>38.65</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>41.54</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>44.94</v>
       </c>
     </row>
@@ -5482,8 +6927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9C89DE-67A8-4D1F-93EB-C3FF4E7F7F64}">
   <dimension ref="B2:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5492,112 +6937,112 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>5000</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>8000</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>10000</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>16000</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>20000</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>40000</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>60000</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>80000</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <v>100000</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>46.34</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>48.29</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>46.86</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>58.39</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>52.9</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>61.04</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>64.209999999999994</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>64.239999999999995</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <v>66.260000000000005</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>45.09</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>43.85</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>42.75</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>51.52</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>47.1</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>51.94</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>54.83</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>62.36</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>61.8</v>
       </c>
     </row>
@@ -5612,15 +7057,133 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E2E635-709C-4E0D-953B-0635311F1154}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5000</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8000</v>
+      </c>
+      <c r="E3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="F3" s="1">
+        <v>16000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>20000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>40000</v>
+      </c>
+      <c r="I3" s="1">
+        <v>60000</v>
+      </c>
+      <c r="J3" s="1">
+        <v>80000</v>
+      </c>
+      <c r="K3" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>52.51</v>
+      </c>
+      <c r="D4" s="1">
+        <v>55.9</v>
+      </c>
+      <c r="E4" s="1">
+        <v>57.95</v>
+      </c>
+      <c r="F4" s="1">
+        <v>72.650000000000006</v>
+      </c>
+      <c r="G4" s="1">
+        <v>60.32</v>
+      </c>
+      <c r="H4" s="1">
+        <v>67.27</v>
+      </c>
+      <c r="I4" s="1">
+        <v>73.78</v>
+      </c>
+      <c r="J4" s="1">
+        <v>66.69</v>
+      </c>
+      <c r="K4" s="1">
+        <v>66.290000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>63.68</v>
+      </c>
+      <c r="D5" s="1">
+        <v>81.39</v>
+      </c>
+      <c r="E5" s="1">
+        <v>84.6</v>
+      </c>
+      <c r="F5" s="1">
+        <v>99.32</v>
+      </c>
+      <c r="G5" s="1">
+        <v>105.94</v>
+      </c>
+      <c r="H5" s="1">
+        <v>144.51</v>
+      </c>
+      <c r="I5" s="1">
+        <v>198.84</v>
+      </c>
+      <c r="J5" s="1">
+        <v>260.05</v>
+      </c>
+      <c r="K5" s="1">
+        <v>260.27999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:K2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5628,8 +7191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF7DADA-17D3-4983-8BCC-287B39656EC3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>